<commit_message>
csv file added logic
</commit_message>
<xml_diff>
--- a/src/test/resources/Hamster.xlsx
+++ b/src/test/resources/Hamster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PORTISHEAD\Desktop\HamsterCount\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A73F74E-C336-4682-8BB7-71CD0721554A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1692F7-9DE7-4F58-89FB-D5B0C48B6378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{0E792634-8D00-4DE1-A122-B28972D8939E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="398" xr2:uid="{0E792634-8D00-4DE1-A122-B28972D8939E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>Markets</t>
   </si>
@@ -62,248 +62,1416 @@
     <t>Coins ballance:</t>
   </si>
   <si>
-    <t>Markets:Fan tokens</t>
-  </si>
-  <si>
-    <t>Markets:Staking</t>
-  </si>
-  <si>
-    <t>Markets:BTC pairs</t>
-  </si>
-  <si>
-    <t>Markets:ETH pairs</t>
-  </si>
-  <si>
-    <t>Markets:Top 10 cmc pairs</t>
-  </si>
-  <si>
-    <t>Markets:GameFi tokens</t>
-  </si>
-  <si>
-    <t>Markets:Defi 2,0 tokens</t>
-  </si>
-  <si>
-    <t>Markets:Social FI tokens</t>
-  </si>
-  <si>
-    <t>Markets:Meme coins</t>
-  </si>
-  <si>
-    <t>Markets:Shit coins</t>
-  </si>
-  <si>
-    <t>Markets:Mergin trading x10</t>
-  </si>
-  <si>
-    <t>Markets:Mergin trading x20</t>
-  </si>
-  <si>
-    <t>Markets:Mergin trading x30</t>
-  </si>
-  <si>
-    <t>Markets:Mergin trading x50</t>
-  </si>
-  <si>
-    <t>Markets:Mergin trading x75</t>
-  </si>
-  <si>
-    <t>Markets:Mergin trading x100</t>
-  </si>
-  <si>
-    <t>Markets:Derivatives</t>
-  </si>
-  <si>
-    <t>Markets:Prediction marcets</t>
-  </si>
-  <si>
-    <t>Markets:Web3 intergration</t>
-  </si>
-  <si>
-    <t>Markets:Markets:DAO</t>
-  </si>
-  <si>
-    <t>Markets:P2P trading</t>
-  </si>
-  <si>
-    <t>Markets:Tradings bots</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Support team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:HamsterBook</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:X</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Cointelegraph</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:HamsterTube</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:HamsterGram</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:TikTok</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Coindesk</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Influenser</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:CEO</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:IT team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Marketing</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Partnership program</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Product team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:BisDev team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Two factor authentication</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:UX &amp; UI team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Security team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:QA team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Antihacking shield</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Risk managment team</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Security Audition</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Ananymous transaction ban</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Blocking suspicious accounts</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Tokenomics expert</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Consensus Explorer pass</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:VC labc</t>
-  </si>
-  <si>
-    <t>PR&amp;Team:Compliance officer</t>
-  </si>
-  <si>
-    <t>Legal:KYC</t>
-  </si>
-  <si>
-    <t>Legal:KYB</t>
-  </si>
-  <si>
-    <t>Legal:Legal opinion</t>
-  </si>
-  <si>
-    <t>Legal:SEC transparancy</t>
-  </si>
-  <si>
-    <t>Legal:Anti money loundering</t>
-  </si>
-  <si>
-    <t>Legal:Licence UAE</t>
-  </si>
-  <si>
-    <t>Legal:Licence Europe</t>
-  </si>
-  <si>
-    <t>Legal:Licence Asia</t>
-  </si>
-  <si>
-    <t>Legal:Licence South America</t>
-  </si>
-  <si>
-    <t>Legal:Licence Australia</t>
-  </si>
-  <si>
-    <t>Legal:Licence North America</t>
-  </si>
-  <si>
-    <t>Legal:Licence Nigeria</t>
-  </si>
-  <si>
-    <t>SPECIALS:TON + Hamster Kombat = Success</t>
-  </si>
-  <si>
-    <t>SPECIALS:Consensus Piranha Pass</t>
-  </si>
-  <si>
-    <t>SPECIALS:Web3 academy launch</t>
-  </si>
-  <si>
-    <t>SPECIALS:YouTube Gold Button</t>
-  </si>
-  <si>
-    <t>SPECIALS:Hamster YouTube Channel</t>
-  </si>
-  <si>
-    <t>SPECIALS:Bitcoin Pizza Day</t>
-  </si>
-  <si>
-    <t>SPECIALS:Top 10 Global Ranking</t>
-  </si>
-  <si>
-    <t>SPECIALS:NFT Collection Launch</t>
-  </si>
-  <si>
-    <t>SPECIALS:Special Hamster Conference</t>
-  </si>
-  <si>
-    <t>SPECIALS:Short squeeze</t>
-  </si>
-  <si>
-    <t>SPECIALS:There are two chairs</t>
-  </si>
-  <si>
-    <t>SPECIALS:Long squeeze</t>
-  </si>
-  <si>
-    <t>SPECIALS:Villa for the DEV team</t>
-  </si>
-  <si>
-    <t>SPECIALS:Apps Center Listing</t>
-  </si>
-  <si>
-    <t>SPECIALS:Bogdanoff is calling</t>
-  </si>
-  <si>
-    <t>SPECIALS:USDT on TON</t>
-  </si>
-  <si>
-    <t>Legal:Licence Japan</t>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Premarket Launch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hamster Kombat merch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TON + Hamster Kombat = Success</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Consensus Piranha Pass</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Web3 academy launch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YouTube Gold Button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hamster YouTube Channel</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bitcoin Pizza Day</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Top 10 Global Ranking</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NFT Collection Launch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Special Hamster Conference</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Short squeeze</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There are two chairs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Long squeeze</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Villa for the DEV team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apps Center Listing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bogdanoff is calling</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SPECIALS:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USDT on TON</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KYC</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KYB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Legal opinion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SEC transparancy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Anti money loundering</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence UAE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence Europe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence Asia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence South America</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence Australia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence North America</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence Nigeria</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence Japan</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Legal:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Licence Ethiopia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mergin trading x20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mergin trading x30</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mergin trading x50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mergin trading x75</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mergin trading x100</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Derivatives</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prediction marcets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Web3 intergration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DAO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P2P trading</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tradings bots</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Support team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HamsterBook</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cointelegraph</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HamsterTube</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HamsterGram</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TikTok</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Coindesk</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Influenser</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CEO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IT team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Marketing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partnership program</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Product team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BisDev team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Two factor authentication</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UX &amp; UI team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Security team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>QA team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Antihacking shield</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Risk managment team</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Security Audition</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ananymous transaction ban</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Blocking suspicious accounts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tokenomics expert</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Consensus Explorer pass</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VC labc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Compliance officer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PR&amp;Team:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Welcome to Amsterdam</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BTC pairs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Staking</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fan tokens</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ETH pairs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Top 10 cmc pairs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GameFi tokens</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Defi 2,0 tokens</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Social FI tokens</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Meme coins</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shit coins</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markets:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mergin trading x10</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +1499,28 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -464,7 +1654,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -501,6 +1691,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -859,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034DAE2C-24FA-401D-B9D1-8F70027E9558}">
-  <dimension ref="A1:BF84"/>
+  <dimension ref="A1:BF88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,7 +2070,7 @@
     <col min="2" max="2" width="10.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
     <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -883,16 +2082,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="14">
-        <v>260877</v>
+        <v>128900000</v>
       </c>
       <c r="F1"/>
       <c r="G1"/>
@@ -963,14 +2162,14 @@
       <c r="I2"/>
     </row>
     <row r="3" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
+      <c r="A3" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="B3" s="2">
-        <v>1590000</v>
+        <v>3322971</v>
       </c>
       <c r="C3" s="2">
-        <v>2280</v>
+        <v>2450</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -1027,22 +2226,22 @@
       <c r="BF3"/>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>9</v>
+      <c r="A4" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="B4" s="4">
-        <v>1160000</v>
+        <v>2538770</v>
       </c>
       <c r="C4" s="4">
-        <v>1540</v>
+        <v>1650</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
     </row>
     <row r="5" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
+      <c r="A5" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="B5" s="2">
         <v>415630</v>
@@ -1107,8 +2306,8 @@
       <c r="BF5"/>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
+      <c r="A6" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="B6" s="4">
         <v>498760</v>
@@ -1123,14 +2322,14 @@
       <c r="I6"/>
     </row>
     <row r="7" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
+      <c r="A7" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="B7" s="2">
-        <v>332297</v>
+        <v>725363</v>
       </c>
       <c r="C7" s="6">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -1189,14 +2388,14 @@
       <c r="BF7"/>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>13</v>
+      <c r="A8" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="B8" s="4">
-        <v>362681</v>
+        <v>831273</v>
       </c>
       <c r="C8" s="3">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
@@ -1205,14 +2404,14 @@
       <c r="I8"/>
     </row>
     <row r="9" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>14</v>
+      <c r="A9" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="B9" s="2">
-        <v>362681</v>
+        <v>831273</v>
       </c>
       <c r="C9" s="6">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -1271,8 +2470,8 @@
       <c r="BF9"/>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>15</v>
+      <c r="A10" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="B10" s="3">
         <v>362681</v>
@@ -1287,14 +2486,14 @@
       <c r="I10"/>
     </row>
     <row r="11" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>16</v>
+      <c r="A11" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="B11" s="6">
-        <v>664594</v>
+        <v>3325090</v>
       </c>
       <c r="C11" s="6">
-        <v>284</v>
+        <v>325</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -1353,14 +2552,14 @@
       <c r="BF11"/>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>17</v>
+      <c r="A12" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="B12" s="3">
-        <v>1661486</v>
+        <v>8312726</v>
       </c>
       <c r="C12" s="3">
-        <v>1520</v>
+        <v>1740</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -1369,14 +2568,14 @@
       <c r="I12"/>
     </row>
     <row r="13" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>18</v>
+      <c r="A13" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="B13" s="6">
-        <v>830743</v>
+        <v>1813407</v>
       </c>
       <c r="C13" s="6">
-        <v>709</v>
+        <v>759</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -1436,13 +2635,13 @@
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3">
-        <v>830743</v>
+        <v>1813407</v>
       </c>
       <c r="C14" s="3">
-        <v>902</v>
+        <v>966</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
@@ -1452,13 +2651,13 @@
     </row>
     <row r="15" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B15" s="6">
-        <v>1160000</v>
+        <v>5818908</v>
       </c>
       <c r="C15" s="6">
-        <v>1280</v>
+        <v>1470</v>
       </c>
       <c r="D15"/>
       <c r="E15"/>
@@ -1518,7 +2717,7 @@
     </row>
     <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3">
         <v>16625452</v>
@@ -1534,13 +2733,13 @@
     </row>
     <row r="17" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B17" s="6">
-        <v>2490000</v>
+        <v>5440222</v>
       </c>
       <c r="C17" s="6">
-        <v>2830</v>
+        <v>3030</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -1600,7 +2799,7 @@
     </row>
     <row r="18" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3">
         <v>3626815</v>
@@ -1616,13 +2815,13 @@
     </row>
     <row r="19" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B19" s="6">
-        <v>1813407</v>
+        <v>4156363</v>
       </c>
       <c r="C19" s="6">
-        <v>1360</v>
+        <v>1460</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -1682,13 +2881,13 @@
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B20" s="3">
-        <v>1269385</v>
+        <v>7001948</v>
       </c>
       <c r="C20" s="3">
-        <v>952</v>
+        <v>1090</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
@@ -1698,13 +2897,13 @@
     </row>
     <row r="21" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B21" s="6">
-        <v>2159931</v>
+        <v>4714859</v>
       </c>
       <c r="C21" s="6">
-        <v>2030</v>
+        <v>2180</v>
       </c>
       <c r="D21"/>
       <c r="E21"/>
@@ -1764,13 +2963,13 @@
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B22" s="3">
-        <v>725363</v>
+        <v>4001113</v>
       </c>
       <c r="C22" s="3">
-        <v>635</v>
+        <v>727</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
@@ -1782,13 +2981,13 @@
     </row>
     <row r="23" spans="1:58" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B23" s="6">
-        <v>671331</v>
+        <v>6982690</v>
       </c>
       <c r="C23" s="6">
-        <v>940</v>
+        <v>1150</v>
       </c>
       <c r="D23"/>
       <c r="E23"/>
@@ -1848,13 +3047,13 @@
     </row>
     <row r="24" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3">
-        <v>697824</v>
+        <v>3491345</v>
       </c>
       <c r="C24" s="3">
-        <v>503</v>
+        <v>576</v>
       </c>
       <c r="D24"/>
       <c r="E24"/>
@@ -1865,11 +3064,11 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="G25"/>
@@ -1880,7 +3079,7 @@
     </row>
     <row r="26" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B26" s="3">
         <v>544020</v>
@@ -1894,7 +3093,7 @@
     </row>
     <row r="27" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B27" s="6">
         <v>362680</v>
@@ -1908,13 +3107,13 @@
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B28" s="3">
-        <v>398950</v>
+        <v>914400</v>
       </c>
       <c r="C28" s="3">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1922,7 +3121,7 @@
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="B29" s="6">
         <v>581890</v>
@@ -1936,29 +3135,29 @@
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B30" s="3">
-        <v>435210</v>
+        <v>2400668</v>
       </c>
       <c r="C30" s="3">
-        <v>248</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B31" s="6">
-        <v>362680</v>
+        <v>831273</v>
       </c>
       <c r="C31" s="6">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B32" s="3">
         <v>544020</v>
@@ -1969,29 +3168,29 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B33" s="6">
-        <v>332290</v>
+        <v>725363</v>
       </c>
       <c r="C33" s="6">
-        <v>206</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B34" s="3">
-        <v>830740</v>
+        <v>4156363</v>
       </c>
       <c r="C34" s="3">
-        <v>696</v>
+        <v>797</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B35" s="6">
         <v>725360</v>
@@ -2002,18 +3201,18 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B36" s="3">
-        <v>664590</v>
+        <v>3325090</v>
       </c>
       <c r="C36" s="3">
-        <v>619</v>
+        <v>709</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B37" s="6">
         <v>332290</v>
@@ -2024,7 +3223,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B38" s="3">
         <v>362680</v>
@@ -2035,18 +3234,18 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B39" s="6">
-        <v>332290</v>
+        <v>1662545</v>
       </c>
       <c r="C39" s="6">
-        <v>258</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B40" s="3">
         <v>362680</v>
@@ -2057,106 +3256,106 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B41" s="6">
-        <v>332290</v>
+        <v>725363</v>
       </c>
       <c r="C41" s="6">
-        <v>322</v>
+        <v>345</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="B42" s="3">
-        <v>551270</v>
+        <v>1263534</v>
       </c>
       <c r="C42" s="3">
-        <v>483</v>
+        <v>517</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B43" s="6">
-        <v>725360</v>
+        <v>1662454</v>
       </c>
       <c r="C43" s="6">
-        <v>552</v>
+        <v>590</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B44" s="3">
-        <v>924830</v>
+        <v>2119745</v>
       </c>
       <c r="C44" s="3">
-        <v>524</v>
+        <v>561</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B45" s="6">
-        <v>319680</v>
+        <v>664594</v>
       </c>
       <c r="C45" s="6">
-        <v>265</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B46" s="3">
-        <v>664590</v>
+        <v>1450726</v>
       </c>
       <c r="C46" s="3">
-        <v>683</v>
+        <v>731</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B47" s="6">
-        <v>479520</v>
+        <v>996891</v>
       </c>
       <c r="C47" s="6">
-        <v>241</v>
+        <v>258</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="B48" s="3">
-        <v>652820</v>
+        <v>1496291</v>
       </c>
       <c r="C48" s="3">
-        <v>828</v>
+        <v>886</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="B49" s="6">
-        <v>415370</v>
+        <v>2078181</v>
       </c>
       <c r="C49" s="6">
-        <v>413</v>
+        <v>472</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B50" s="3">
         <v>1661486</v>
@@ -2167,29 +3366,29 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B51" s="6">
-        <v>3990000</v>
+        <v>8307428</v>
       </c>
       <c r="C51" s="6">
-        <v>3610</v>
+        <v>3860</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B52" s="3">
-        <v>1251321</v>
+        <v>2477529</v>
       </c>
       <c r="C52" s="3">
-        <v>1120</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B53" s="6">
         <v>559440</v>
@@ -2199,335 +3398,379 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="15">
+        <v>479522</v>
+      </c>
+      <c r="C54" s="15">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="13">
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="13">
         <v>400110</v>
       </c>
-      <c r="C55" s="13">
+      <c r="C56" s="13">
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="3">
         <v>362680</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C57" s="3">
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="13">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="13">
         <v>332290</v>
       </c>
-      <c r="C57" s="13">
+      <c r="C58" s="13">
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="3">
         <v>398750</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C59" s="3">
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="13">
-        <v>479520</v>
-      </c>
-      <c r="C59" s="13">
-        <v>675</v>
-      </c>
-    </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B60" s="3">
+      <c r="A60" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="13">
+        <v>996891</v>
+      </c>
+      <c r="C60" s="13">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="3">
         <v>3620000</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C61" s="3">
         <v>1540</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" s="13">
-        <v>1660000</v>
-      </c>
-      <c r="C61" s="13">
-        <v>1850</v>
-      </c>
-    </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="3">
-        <v>799200</v>
-      </c>
-      <c r="C62" s="3">
-        <v>892</v>
+      <c r="A62" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="13">
+        <v>8312726</v>
+      </c>
+      <c r="C62" s="13">
+        <v>2120</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="13">
-        <v>799203</v>
-      </c>
-      <c r="C63" s="13">
-        <v>940</v>
+      <c r="A63" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="3">
+        <v>3626815</v>
+      </c>
+      <c r="C63" s="3">
+        <v>1020</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="3">
-        <v>1660000</v>
-      </c>
-      <c r="C64" s="3">
-        <v>1750</v>
+      <c r="A64" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="13">
+        <v>1661486</v>
+      </c>
+      <c r="C64" s="13">
+        <v>1000</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="13">
+      <c r="A65" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="3">
+        <v>3626815</v>
+      </c>
+      <c r="C65" s="3">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="13">
         <v>3320000</v>
       </c>
-      <c r="C65" s="13">
+      <c r="C66" s="13">
         <v>2470</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="3">
-        <v>498440</v>
-      </c>
-      <c r="C66" s="3">
-        <v>438</v>
-      </c>
-    </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67" s="6">
-        <v>696930</v>
-      </c>
-      <c r="C67" s="6">
-        <v>4780</v>
+      <c r="A67" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1088044</v>
+      </c>
+      <c r="C67" s="3">
+        <v>469</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
+      <c r="A68" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="6">
+        <v>16614856</v>
+      </c>
+      <c r="C68" s="6">
+        <v>6700</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B69" s="3">
-        <v>5510000</v>
+        <v>5594421</v>
       </c>
       <c r="C69" s="3">
-        <v>8020</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" s="6">
-        <v>4030000</v>
-      </c>
-      <c r="C70" s="6">
-        <v>4270</v>
-      </c>
+      <c r="A70" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B71" s="3">
-        <v>3650000</v>
-      </c>
-      <c r="C71" s="3">
-        <v>3860</v>
+        <v>8</v>
+      </c>
+      <c r="B71" s="4">
+        <v>13938696</v>
+      </c>
+      <c r="C71" s="4">
+        <v>13780</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="B72" s="6">
-        <v>830743</v>
+        <v>242191</v>
       </c>
       <c r="C72" s="6">
-        <v>709</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="B73" s="3">
-        <v>498440</v>
+        <v>13938696</v>
       </c>
       <c r="C73" s="3">
-        <v>645</v>
+        <v>9190</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="B74" s="6">
-        <v>725360</v>
+        <v>7992030</v>
       </c>
       <c r="C74" s="6">
-        <v>276</v>
+        <v>4570</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B75" s="3">
-        <v>7250000</v>
+        <v>7978993</v>
       </c>
       <c r="C75" s="3">
-        <v>3310</v>
+        <v>4130</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="B76" s="6">
-        <v>5640000</v>
+        <v>4156363</v>
       </c>
       <c r="C76" s="6">
-        <v>3090</v>
+        <v>812</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B77" s="3">
-        <v>1660000</v>
+        <v>1088044</v>
       </c>
       <c r="C77" s="3">
-        <v>2320</v>
+        <v>690</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="B78" s="6">
-        <v>2820000</v>
+        <v>725360</v>
       </c>
       <c r="C78" s="6">
-        <v>2250</v>
+        <v>276</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="B79" s="3">
-        <v>4030000</v>
+        <v>16625452</v>
       </c>
       <c r="C79" s="3">
-        <v>4500</v>
+        <v>3540</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="B80" s="6">
-        <v>9960000</v>
+        <v>12331170</v>
       </c>
       <c r="C80" s="6">
-        <v>5150</v>
+        <v>3310</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B81" s="3">
-        <v>3320000</v>
+        <v>3626815</v>
       </c>
       <c r="C81" s="3">
-        <v>1320</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B82" s="6">
-        <v>2390000</v>
+        <v>2820000</v>
       </c>
       <c r="C82" s="6">
-        <v>2410</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B83" s="3">
-        <v>799200</v>
+        <v>7992030</v>
       </c>
       <c r="C83" s="3">
-        <v>1140</v>
+        <v>4820</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="B84" s="6">
+        <v>9960000</v>
+      </c>
+      <c r="C84" s="6">
+        <v>5150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85" s="3">
+        <v>3320000</v>
+      </c>
+      <c r="C85" s="3">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="6">
+        <v>10880444</v>
+      </c>
+      <c r="C86" s="6">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1661486</v>
+      </c>
+      <c r="C87" s="3">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B88" s="6">
         <v>7250000</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C88" s="6">
         <v>3720</v>
       </c>
     </row>
@@ -2535,8 +3778,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A70:C70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>